<commit_message>
some data analysis questions
</commit_message>
<xml_diff>
--- a/EmployeeSQL/Initial Model.xlsx
+++ b/EmployeeSQL/Initial Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noctura\RICE\HomeworkMASTER\RICE-SQL-Challenge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noctura\RICE\HomeworkMASTER\RICE-SQL-Challenge\EmployeeSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7699F3-CC5A-4F0C-992F-989CBEB93044}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648C4D7B-AF1B-495F-89B6-BEA8EC79DAAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B293654E-1825-46D5-8637-44300DA6ECD8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B293654E-1825-46D5-8637-44300DA6ECD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t>dept_emp</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>FK -&lt; titles.title_id</t>
+  </si>
+  <si>
+    <t>DATE</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D34" sqref="D1:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -594,11 +597,11 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">birth_date VARCHAR(30) </v>
+        <v xml:space="preserve">birth_date DATE </v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
@@ -642,11 +645,11 @@
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">hire_date VARCHAR(30) </v>
+        <v xml:space="preserve">hire_date DATE </v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>